<commit_message>
added netbeans centrality plot
</commit_message>
<xml_diff>
--- a/eclipse/correlation/correlation_eclipse_1_10.xlsx
+++ b/eclipse/correlation/correlation_eclipse_1_10.xlsx
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:O92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3:G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1137,12 +1137,12 @@
         <v>19</v>
       </c>
       <c r="G3" s="0" t="n">
-        <f aca="false">((-0.078)*B3+(-0.218)*C3+(-0.477)*E3+(0.227)*F3)/(-0.546)</f>
-        <v>0.0245908058608059</v>
+        <f aca="false">((0.078)*B3+(0.218)*C3+(0.477)*E3+(0.227)*F3)/(1)</f>
+        <v>0.0340745</v>
       </c>
       <c r="H3" s="0" t="n">
-        <f aca="false">((-0.078)*B3+(-0.207)*D3+(-0.477)*E3+(0.227)*F3)/ (-0.535)</f>
-        <v>0.0232686728971963</v>
+        <f aca="false">((0.078)*B3+(0.207)*D3+(0.477)*E3+(0.227)*F3)/ (0.989)</f>
+        <v>0.0334647724974722</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>1176.67444444444</v>
@@ -1186,12 +1186,12 @@
         <v>24</v>
       </c>
       <c r="G4" s="0" t="n">
-        <f aca="false">((-0.078)*B4+(-0.218)*C4+(-0.477)*E4+(0.227)*F4)/(-0.546)</f>
-        <v>0.107506575091575</v>
+        <f aca="false">((0.078)*B4+(0.218)*C4+(0.477)*E4+(0.227)*F4)/(1)</f>
+        <v>0.07973695</v>
       </c>
       <c r="H4" s="0" t="n">
-        <f aca="false">((-0.078)*B4+(-0.207)*D4+(-0.477)*E4+(0.227)*F4)/ (-0.535)</f>
-        <v>0.0817431401869159</v>
+        <f aca="false">((0.078)*B4+(0.207)*D4+(0.477)*E4+(0.227)*F4)/ (0.989)</f>
+        <v>0.0654913447927199</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>1652.21944444444</v>
@@ -1235,12 +1235,12 @@
         <v>29</v>
       </c>
       <c r="G5" s="0" t="n">
-        <f aca="false">((-0.078)*B5+(-0.218)*C5+(-0.477)*E5+(0.227)*F5)/(-0.546)</f>
-        <v>0.082090347985348</v>
+        <f aca="false">((0.078)*B5+(0.218)*C5+(0.477)*E5+(0.227)*F5)/(1)</f>
+        <v>0.06586877</v>
       </c>
       <c r="H5" s="0" t="n">
-        <f aca="false">((-0.078)*B5+(-0.207)*D5+(-0.477)*E5+(0.227)*F5)/ (-0.535)</f>
-        <v>0.105386429906542</v>
+        <f aca="false">((0.078)*B5+(0.207)*D5+(0.477)*E5+(0.227)*F5)/ (0.989)</f>
+        <v>0.0782903741152679</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>1484.05444444444</v>
@@ -1284,12 +1284,12 @@
         <v>34</v>
       </c>
       <c r="G6" s="0" t="n">
-        <f aca="false">((-0.078)*B6+(-0.218)*C6+(-0.477)*E6+(0.227)*F6)/(-0.546)</f>
-        <v>0.0216627838827839</v>
+        <f aca="false">((0.078)*B6+(0.218)*C6+(0.477)*E6+(0.227)*F6)/(1)</f>
+        <v>0.03212622</v>
       </c>
       <c r="H6" s="0" t="n">
-        <f aca="false">((-0.078)*B6+(-0.207)*D6+(-0.477)*E6+(0.227)*F6)/ (-0.535)</f>
-        <v>0.0427945420560748</v>
+        <f aca="false">((0.078)*B6+(0.207)*D6+(0.477)*E6+(0.227)*F6)/ (0.989)</f>
+        <v>0.0436738321536906</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>431.345555555556</v>
@@ -1333,12 +1333,12 @@
         <v>39</v>
       </c>
       <c r="G7" s="0" t="n">
-        <f aca="false">((-0.078)*B7+(-0.218)*C7+(-0.477)*E7+(0.227)*F7)/(-0.546)</f>
-        <v>-0.00394553113553113</v>
+        <f aca="false">((0.078)*B7+(0.218)*C7+(0.477)*E7+(0.227)*F7)/(1)</f>
+        <v>0.0181577</v>
       </c>
       <c r="H7" s="0" t="n">
-        <f aca="false">((-0.078)*B7+(-0.207)*D7+(-0.477)*E7+(0.227)*F7)/ (-0.535)</f>
-        <v>-0.00165351401869159</v>
+        <f aca="false">((0.078)*B7+(0.207)*D7+(0.477)*E7+(0.227)*F7)/ (0.989)</f>
+        <v>0.0196434074823054</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>957.875555555556</v>
@@ -1382,12 +1382,12 @@
         <v>44</v>
       </c>
       <c r="G8" s="0" t="n">
-        <f aca="false">((-0.078)*B8+(-0.218)*C8+(-0.477)*E8+(0.227)*F8)/(-0.546)</f>
-        <v>0.137101446886447</v>
+        <f aca="false">((0.078)*B8+(0.218)*C8+(0.477)*E8+(0.227)*F8)/(1)</f>
+        <v>0.09600925</v>
       </c>
       <c r="H8" s="0" t="n">
-        <f aca="false">((-0.078)*B8+(-0.207)*D8+(-0.477)*E8+(0.227)*F8)/ (-0.535)</f>
-        <v>0.124225457943925</v>
+        <f aca="false">((0.078)*B8+(0.207)*D8+(0.477)*E8+(0.227)*F8)/ (0.989)</f>
+        <v>0.0885869362992922</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>514.827777777778</v>
@@ -1431,12 +1431,12 @@
         <v>49</v>
       </c>
       <c r="G9" s="0" t="n">
-        <f aca="false">((-0.078)*B9+(-0.218)*C9+(-0.477)*E9+(0.227)*F9)/(-0.546)</f>
-        <v>0.0683762454212454</v>
+        <f aca="false">((0.078)*B9+(0.218)*C9+(0.477)*E9+(0.227)*F9)/(1)</f>
+        <v>0.05849891</v>
       </c>
       <c r="H9" s="0" t="n">
-        <f aca="false">((-0.078)*B9+(-0.207)*D9+(-0.477)*E9+(0.227)*F9)/ (-0.535)</f>
-        <v>0.0909394205607477</v>
+        <f aca="false">((0.078)*B9+(0.207)*D9+(0.477)*E9+(0.227)*F9)/ (0.989)</f>
+        <v>0.0705946107178969</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>1544.77805555556</v>
@@ -1480,12 +1480,12 @@
         <v>54</v>
       </c>
       <c r="G10" s="0" t="n">
-        <f aca="false">((-0.078)*B10+(-0.218)*C10+(-0.477)*E10+(0.227)*F10)/(-0.546)</f>
-        <v>0.0686104395604396</v>
+        <f aca="false">((0.078)*B10+(0.218)*C10+(0.477)*E10+(0.227)*F10)/(1)</f>
+        <v>0.05849058</v>
       </c>
       <c r="H10" s="0" t="n">
-        <f aca="false">((-0.078)*B10+(-0.207)*D10+(-0.477)*E10+(0.227)*F10)/ (-0.535)</f>
-        <v>0.0704165607476635</v>
+        <f aca="false">((0.078)*B10+(0.207)*D10+(0.477)*E10+(0.227)*F10)/ (0.989)</f>
+        <v>0.0593550455005056</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>1889.70083333333</v>
@@ -1529,12 +1529,12 @@
         <v>59</v>
       </c>
       <c r="G11" s="0" t="n">
-        <f aca="false">((-0.078)*B11+(-0.218)*C11+(-0.477)*E11+(0.227)*F11)/(-0.546)</f>
-        <v>0.0750230036630037</v>
+        <f aca="false">((0.078)*B11+(0.218)*C11+(0.477)*E11+(0.227)*F11)/(1)</f>
+        <v>0.06206448</v>
       </c>
       <c r="H11" s="0" t="n">
-        <f aca="false">((-0.078)*B11+(-0.207)*D11+(-0.477)*E11+(0.227)*F11)/ (-0.535)</f>
-        <v>0.0616711588785047</v>
+        <f aca="false">((0.078)*B11+(0.207)*D11+(0.477)*E11+(0.227)*F11)/ (0.989)</f>
+        <v>0.0546976643073812</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>93.6361111111111</v>
@@ -1578,12 +1578,12 @@
         <v>64</v>
       </c>
       <c r="G12" s="0" t="n">
-        <f aca="false">((-0.078)*B12+(-0.218)*C12+(-0.477)*E12+(0.227)*F12)/(-0.546)</f>
-        <v>0.0663215567765568</v>
+        <f aca="false">((0.078)*B12+(0.218)*C12+(0.477)*E12+(0.227)*F12)/(1)</f>
+        <v>0.05736797</v>
       </c>
       <c r="H12" s="0" t="n">
-        <f aca="false">((-0.078)*B12+(-0.207)*D12+(-0.477)*E12+(0.227)*F12)/ (-0.535)</f>
-        <v>0.0591525607476636</v>
+        <f aca="false">((0.078)*B12+(0.207)*D12+(0.477)*E12+(0.227)*F12)/ (0.989)</f>
+        <v>0.0533903134479272</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>1907.7775</v>
@@ -1627,12 +1627,12 @@
         <v>68</v>
       </c>
       <c r="G13" s="0" t="n">
-        <f aca="false">((-0.078)*B13+(-0.218)*C13+(-0.477)*E13+(0.227)*F13)/(-0.546)</f>
-        <v>-0.00608798534798535</v>
+        <f aca="false">((0.078)*B13+(0.218)*C13+(0.477)*E13+(0.227)*F13)/(1)</f>
+        <v>0.01726486</v>
       </c>
       <c r="H13" s="0" t="n">
-        <f aca="false">((-0.078)*B13+(-0.207)*D13+(-0.477)*E13+(0.227)*F13)/ (-0.535)</f>
-        <v>-0.00366977570093458</v>
+        <f aca="false">((0.078)*B13+(0.207)*D13+(0.477)*E13+(0.227)*F13)/ (0.989)</f>
+        <v>0.0188327300303337</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>1238.45694444444</v>
@@ -1676,12 +1676,12 @@
         <v>73</v>
       </c>
       <c r="G14" s="0" t="n">
-        <f aca="false">((-0.078)*B14+(-0.218)*C14+(-0.477)*E14+(0.227)*F14)/(-0.546)</f>
-        <v>0.0518550915750916</v>
+        <f aca="false">((0.078)*B14+(0.218)*C14+(0.477)*E14+(0.227)*F14)/(1)</f>
+        <v>0.0489154</v>
       </c>
       <c r="H14" s="0" t="n">
-        <f aca="false">((-0.078)*B14+(-0.207)*D14+(-0.477)*E14+(0.227)*F14)/ (-0.535)</f>
-        <v>0.0494382429906542</v>
+        <f aca="false">((0.078)*B14+(0.207)*D14+(0.477)*E14+(0.227)*F14)/ (0.989)</f>
+        <v>0.0475753083923155</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>1068.9775</v>
@@ -1725,12 +1725,12 @@
         <v>78</v>
       </c>
       <c r="G15" s="0" t="n">
-        <f aca="false">((-0.078)*B15+(-0.218)*C15+(-0.477)*E15+(0.227)*F15)/(-0.546)</f>
-        <v>0.0642237362637363</v>
+        <f aca="false">((0.078)*B15+(0.218)*C15+(0.477)*E15+(0.227)*F15)/(1)</f>
+        <v>0.05322162</v>
       </c>
       <c r="H15" s="0" t="n">
-        <f aca="false">((-0.078)*B15+(-0.207)*D15+(-0.477)*E15+(0.227)*F15)/ (-0.535)</f>
-        <v>0.0667326728971963</v>
+        <f aca="false">((0.078)*B15+(0.207)*D15+(0.477)*E15+(0.227)*F15)/ (0.989)</f>
+        <v>0.0544564610717897</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>476.525277777778</v>
@@ -1774,12 +1774,12 @@
         <v>78</v>
       </c>
       <c r="G16" s="0" t="n">
-        <f aca="false">((-0.078)*B16+(-0.218)*C16+(-0.477)*E16+(0.227)*F16)/(-0.546)</f>
-        <v>0.0628916483516484</v>
+        <f aca="false">((0.078)*B16+(0.218)*C16+(0.477)*E16+(0.227)*F16)/(1)</f>
+        <v>0.0524943</v>
       </c>
       <c r="H16" s="0" t="n">
-        <f aca="false">((-0.078)*B16+(-0.207)*D16+(-0.477)*E16+(0.227)*F16)/ (-0.535)</f>
-        <v>0.0654428411214953</v>
+        <f aca="false">((0.078)*B16+(0.207)*D16+(0.477)*E16+(0.227)*F16)/ (0.989)</f>
+        <v>0.0537587259858443</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>372.477777777778</v>
@@ -1823,12 +1823,12 @@
         <v>85</v>
       </c>
       <c r="G17" s="0" t="n">
-        <f aca="false">((-0.078)*B17+(-0.218)*C17+(-0.477)*E17+(0.227)*F17)/(-0.546)</f>
-        <v>0.0982668864468864</v>
+        <f aca="false">((0.078)*B17+(0.218)*C17+(0.477)*E17+(0.227)*F17)/(1)</f>
+        <v>0.07128254</v>
       </c>
       <c r="H17" s="0" t="n">
-        <f aca="false">((-0.078)*B17+(-0.207)*D17+(-0.477)*E17+(0.227)*F17)/ (-0.535)</f>
-        <v>0.101440953271028</v>
+        <f aca="false">((0.078)*B17+(0.207)*D17+(0.477)*E17+(0.227)*F17)/ (0.989)</f>
+        <v>0.0726994236602629</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>560.1675</v>
@@ -1872,12 +1872,12 @@
         <v>89</v>
       </c>
       <c r="G18" s="0" t="n">
-        <f aca="false">((-0.078)*B18+(-0.218)*C18+(-0.477)*E18+(0.227)*F18)/(-0.546)</f>
-        <v>0.101464798534799</v>
+        <f aca="false">((0.078)*B18+(0.218)*C18+(0.477)*E18+(0.227)*F18)/(1)</f>
+        <v>0.07399562</v>
       </c>
       <c r="H18" s="0" t="n">
-        <f aca="false">((-0.078)*B18+(-0.207)*D18+(-0.477)*E18+(0.227)*F18)/ (-0.535)</f>
-        <v>0.105962093457944</v>
+        <f aca="false">((0.078)*B18+(0.207)*D18+(0.477)*E18+(0.227)*F18)/ (0.989)</f>
+        <v>0.0761229120323559</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>187.720555555556</v>
@@ -1921,12 +1921,12 @@
         <v>93</v>
       </c>
       <c r="G19" s="0" t="n">
-        <f aca="false">((-0.078)*B19+(-0.218)*C19+(-0.477)*E19+(0.227)*F19)/(-0.546)</f>
-        <v>0.0590727655677656</v>
+        <f aca="false">((0.078)*B19+(0.218)*C19+(0.477)*E19+(0.227)*F19)/(1)</f>
+        <v>0.04931051</v>
       </c>
       <c r="H19" s="0" t="n">
-        <f aca="false">((-0.078)*B19+(-0.207)*D19+(-0.477)*E19+(0.227)*F19)/ (-0.535)</f>
-        <v>0.0608722056074766</v>
+        <f aca="false">((0.078)*B19+(0.207)*D19+(0.477)*E19+(0.227)*F19)/ (0.989)</f>
+        <v>0.0501753387259859</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>1873.18194444445</v>
@@ -1970,12 +1970,12 @@
         <v>85</v>
       </c>
       <c r="G20" s="0" t="n">
-        <f aca="false">((-0.078)*B20+(-0.218)*C20+(-0.477)*E20+(0.227)*F20)/(-0.546)</f>
-        <v>0.101108424908425</v>
+        <f aca="false">((0.078)*B20+(0.218)*C20+(0.477)*E20+(0.227)*F20)/(1)</f>
+        <v>0.07283402</v>
       </c>
       <c r="H20" s="0" t="n">
-        <f aca="false">((-0.078)*B20+(-0.207)*D20+(-0.477)*E20+(0.227)*F20)/ (-0.535)</f>
-        <v>0.104557588785047</v>
+        <f aca="false">((0.078)*B20+(0.207)*D20+(0.477)*E20+(0.227)*F20)/ (0.989)</f>
+        <v>0.0743853690596562</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>650.134444444444</v>
@@ -2019,12 +2019,12 @@
         <v>44</v>
       </c>
       <c r="G21" s="0" t="n">
-        <f aca="false">((-0.078)*B21+(-0.218)*C21+(-0.477)*E21+(0.227)*F21)/(-0.546)</f>
-        <v>0.103817362637363</v>
+        <f aca="false">((0.078)*B21+(0.218)*C21+(0.477)*E21+(0.227)*F21)/(1)</f>
+        <v>0.07783614</v>
       </c>
       <c r="H21" s="0" t="n">
-        <f aca="false">((-0.078)*B21+(-0.207)*D21+(-0.477)*E21+(0.227)*F21)/ (-0.535)</f>
-        <v>0.108479102803738</v>
+        <f aca="false">((0.078)*B21+(0.207)*D21+(0.477)*E21+(0.227)*F21)/ (0.989)</f>
+        <v>0.0800689383215369</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>1183.18944444444</v>
@@ -2068,12 +2068,12 @@
         <v>78</v>
       </c>
       <c r="G22" s="0" t="n">
-        <f aca="false">((-0.078)*B22+(-0.218)*C22+(-0.477)*E22+(0.227)*F22)/(-0.546)</f>
-        <v>0.0641052014652015</v>
+        <f aca="false">((0.078)*B22+(0.218)*C22+(0.477)*E22+(0.227)*F22)/(1)</f>
+        <v>0.0531569</v>
       </c>
       <c r="H22" s="0" t="n">
-        <f aca="false">((-0.078)*B22+(-0.207)*D22+(-0.477)*E22+(0.227)*F22)/ (-0.535)</f>
-        <v>0.0665698878504673</v>
+        <f aca="false">((0.078)*B22+(0.207)*D22+(0.477)*E22+(0.227)*F22)/ (0.989)</f>
+        <v>0.0543684024266936</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>313.629722222222</v>
@@ -2117,12 +2117,12 @@
         <v>29</v>
       </c>
       <c r="G23" s="0" t="n">
-        <f aca="false">((-0.078)*B23+(-0.218)*C23+(-0.477)*E23+(0.227)*F23)/(-0.546)</f>
-        <v>0.0618586813186813</v>
+        <f aca="false">((0.078)*B23+(0.218)*C23+(0.477)*E23+(0.227)*F23)/(1)</f>
+        <v>0.05482228</v>
       </c>
       <c r="H23" s="0" t="n">
-        <f aca="false">((-0.078)*B23+(-0.207)*D23+(-0.477)*E23+(0.227)*F23)/ (-0.535)</f>
-        <v>0.0626862242990654</v>
+        <f aca="false">((0.078)*B23+(0.207)*D23+(0.477)*E23+(0.227)*F23)/ (0.989)</f>
+        <v>0.055191678463094</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>488.633333333333</v>
@@ -2166,12 +2166,12 @@
         <v>111</v>
       </c>
       <c r="G24" s="0" t="n">
-        <f aca="false">((-0.078)*B24+(-0.218)*C24+(-0.477)*E24+(0.227)*F24)/(-0.546)</f>
-        <v>-0.0140111538461538</v>
+        <f aca="false">((0.078)*B24+(0.218)*C24+(0.477)*E24+(0.227)*F24)/(1)</f>
+        <v>0.01308863</v>
       </c>
       <c r="H24" s="0" t="n">
-        <f aca="false">((-0.078)*B24+(-0.207)*D24+(-0.477)*E24+(0.227)*F24)/ (-0.535)</f>
-        <v>-0.0161188785046729</v>
+        <f aca="false">((0.078)*B24+(0.207)*D24+(0.477)*E24+(0.227)*F24)/ (0.989)</f>
+        <v>0.012249868554095</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>1407.67694444444</v>
@@ -2215,12 +2215,12 @@
         <v>54</v>
       </c>
       <c r="G25" s="0" t="n">
-        <f aca="false">((-0.078)*B25+(-0.218)*C25+(-0.477)*E25+(0.227)*F25)/(-0.546)</f>
-        <v>0.100908186813187</v>
+        <f aca="false">((0.078)*B25+(0.218)*C25+(0.477)*E25+(0.227)*F25)/(1)</f>
+        <v>0.07612515</v>
       </c>
       <c r="H25" s="0" t="n">
-        <f aca="false">((-0.078)*B25+(-0.207)*D25+(-0.477)*E25+(0.227)*F25)/ (-0.535)</f>
-        <v>0.105316654205607</v>
+        <f aca="false">((0.078)*B25+(0.207)*D25+(0.477)*E25+(0.227)*F25)/ (0.989)</f>
+        <v>0.0782342669362993</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>277.892777777778</v>
@@ -2264,12 +2264,12 @@
         <v>68</v>
       </c>
       <c r="G26" s="0" t="n">
-        <f aca="false">((-0.078)*B26+(-0.218)*C26+(-0.477)*E26+(0.227)*F26)/(-0.546)</f>
-        <v>0.0617824908424909</v>
+        <f aca="false">((0.078)*B26+(0.218)*C26+(0.477)*E26+(0.227)*F26)/(1)</f>
+        <v>0.05432214</v>
       </c>
       <c r="H26" s="0" t="n">
-        <f aca="false">((-0.078)*B26+(-0.207)*D26+(-0.477)*E26+(0.227)*F26)/ (-0.535)</f>
-        <v>0.0622880560747664</v>
+        <f aca="false">((0.078)*B26+(0.207)*D26+(0.477)*E26+(0.227)*F26)/ (0.989)</f>
+        <v>0.054512649140546</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>1293.74111111111</v>
@@ -2313,12 +2313,12 @@
         <v>54</v>
       </c>
       <c r="G27" s="0" t="n">
-        <f aca="false">((-0.078)*B27+(-0.218)*C27+(-0.477)*E27+(0.227)*F27)/(-0.546)</f>
-        <v>0.0985279487179487</v>
+        <f aca="false">((0.078)*B27+(0.218)*C27+(0.477)*E27+(0.227)*F27)/(1)</f>
+        <v>0.07482554</v>
       </c>
       <c r="H27" s="0" t="n">
-        <f aca="false">((-0.078)*B27+(-0.207)*D27+(-0.477)*E27+(0.227)*F27)/ (-0.535)</f>
-        <v>0.101897719626168</v>
+        <f aca="false">((0.078)*B27+(0.207)*D27+(0.477)*E27+(0.227)*F27)/ (0.989)</f>
+        <v>0.0763847927199191</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>386.509444444445</v>
@@ -2362,12 +2362,12 @@
         <v>34</v>
       </c>
       <c r="G28" s="0" t="n">
-        <f aca="false">((-0.078)*B28+(-0.218)*C28+(-0.477)*E28+(0.227)*F28)/(-0.546)</f>
-        <v>-0.00848516483516484</v>
+        <f aca="false">((0.078)*B28+(0.218)*C28+(0.477)*E28+(0.227)*F28)/(1)</f>
+        <v>0.01566544</v>
       </c>
       <c r="H28" s="0" t="n">
-        <f aca="false">((-0.078)*B28+(-0.207)*D28+(-0.477)*E28+(0.227)*F28)/ (-0.535)</f>
-        <v>-0.0108095700934579</v>
+        <f aca="false">((0.078)*B28+(0.207)*D28+(0.477)*E28+(0.227)*F28)/ (0.989)</f>
+        <v>0.0146766632962589</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>3643.23416666667</v>
@@ -2411,12 +2411,12 @@
         <v>93</v>
       </c>
       <c r="G29" s="0" t="n">
-        <f aca="false">((-0.078)*B29+(-0.218)*C29+(-0.477)*E29+(0.227)*F29)/(-0.546)</f>
-        <v>0.0600799633699634</v>
+        <f aca="false">((0.078)*B29+(0.218)*C29+(0.477)*E29+(0.227)*F29)/(1)</f>
+        <v>0.04986044</v>
       </c>
       <c r="H29" s="0" t="n">
-        <f aca="false">((-0.078)*B29+(-0.207)*D29+(-0.477)*E29+(0.227)*F29)/ (-0.535)</f>
-        <v>0.0624688785046729</v>
+        <f aca="false">((0.078)*B29+(0.207)*D29+(0.477)*E29+(0.227)*F29)/ (0.989)</f>
+        <v>0.0510390596562184</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>368.312777777778</v>
@@ -2460,12 +2460,12 @@
         <v>130</v>
       </c>
       <c r="G30" s="0" t="n">
-        <f aca="false">((-0.078)*B30+(-0.218)*C30+(-0.477)*E30+(0.227)*F30)/(-0.546)</f>
-        <v>0.000140567765567763</v>
+        <f aca="false">((0.078)*B30+(0.218)*C30+(0.477)*E30+(0.227)*F30)/(1)</f>
+        <v>0.02046589</v>
       </c>
       <c r="H30" s="0" t="n">
-        <f aca="false">((-0.078)*B30+(-0.207)*D30+(-0.477)*E30+(0.227)*F30)/ (-0.535)</f>
-        <v>0.000880542056074764</v>
+        <f aca="false">((0.078)*B30+(0.207)*D30+(0.477)*E30+(0.227)*F30)/ (0.989)</f>
+        <v>0.0210922446916077</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>3031.27638888889</v>
@@ -2509,12 +2509,12 @@
         <v>111</v>
       </c>
       <c r="G31" s="0" t="n">
-        <f aca="false">((-0.078)*B31+(-0.218)*C31+(-0.477)*E31+(0.227)*F31)/(-0.546)</f>
-        <v>0.0667143223443223</v>
+        <f aca="false">((0.078)*B31+(0.218)*C31+(0.477)*E31+(0.227)*F31)/(1)</f>
+        <v>0.05716474</v>
       </c>
       <c r="H31" s="0" t="n">
-        <f aca="false">((-0.078)*B31+(-0.207)*D31+(-0.477)*E31+(0.227)*F31)/ (-0.535)</f>
-        <v>0.0660824112149533</v>
+        <f aca="false">((0.078)*B31+(0.207)*D31+(0.477)*E31+(0.227)*F31)/ (0.989)</f>
+        <v>0.0567166936299292</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>368.200833333333</v>
@@ -2558,12 +2558,12 @@
         <v>78</v>
       </c>
       <c r="G32" s="0" t="n">
-        <f aca="false">((-0.078)*B32+(-0.218)*C32+(-0.477)*E32+(0.227)*F32)/(-0.546)</f>
-        <v>0.063938021978022</v>
+        <f aca="false">((0.078)*B32+(0.218)*C32+(0.477)*E32+(0.227)*F32)/(1)</f>
+        <v>0.05306562</v>
       </c>
       <c r="H32" s="0" t="n">
-        <f aca="false">((-0.078)*B32+(-0.207)*D32+(-0.477)*E32+(0.227)*F32)/ (-0.535)</f>
-        <v>0.0646767476635514</v>
+        <f aca="false">((0.078)*B32+(0.207)*D32+(0.477)*E32+(0.227)*F32)/ (0.989)</f>
+        <v>0.0533443073811931</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>421.091111111111</v>
@@ -2607,12 +2607,12 @@
         <v>89</v>
       </c>
       <c r="G33" s="0" t="n">
-        <f aca="false">((-0.078)*B33+(-0.218)*C33+(-0.477)*E33+(0.227)*F33)/(-0.546)</f>
-        <v>0.0683947435897436</v>
+        <f aca="false">((0.078)*B33+(0.218)*C33+(0.477)*E33+(0.227)*F33)/(1)</f>
+        <v>0.05593937</v>
       </c>
       <c r="H33" s="0" t="n">
-        <f aca="false">((-0.078)*B33+(-0.207)*D33+(-0.477)*E33+(0.227)*F33)/ (-0.535)</f>
-        <v>0.0719722056074766</v>
+        <f aca="false">((0.078)*B33+(0.207)*D33+(0.477)*E33+(0.227)*F33)/ (0.989)</f>
+        <v>0.0577360667340748</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>226.414722222222</v>
@@ -2656,12 +2656,12 @@
         <v>64</v>
       </c>
       <c r="G34" s="0" t="n">
-        <f aca="false">((-0.078)*B34+(-0.218)*C34+(-0.477)*E34+(0.227)*F34)/(-0.546)</f>
-        <v>0.0198682600732601</v>
+        <f aca="false">((0.078)*B34+(0.218)*C34+(0.477)*E34+(0.227)*F34)/(1)</f>
+        <v>0.03200447</v>
       </c>
       <c r="H34" s="0" t="n">
-        <f aca="false">((-0.078)*B34+(-0.207)*D34+(-0.477)*E34+(0.227)*F34)/ (-0.535)</f>
-        <v>0.0209183177570093</v>
+        <f aca="false">((0.078)*B34+(0.207)*D34+(0.477)*E34+(0.227)*F34)/ (0.989)</f>
+        <v>0.032707482305359</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>2865.90166666667</v>
@@ -2705,12 +2705,12 @@
         <v>111</v>
       </c>
       <c r="G35" s="0" t="n">
-        <f aca="false">((-0.078)*B35+(-0.218)*C35+(-0.477)*E35+(0.227)*F35)/(-0.546)</f>
-        <v>0.0852592857142857</v>
+        <f aca="false">((0.078)*B35+(0.218)*C35+(0.477)*E35+(0.227)*F35)/(1)</f>
+        <v>0.06729029</v>
       </c>
       <c r="H35" s="0" t="n">
-        <f aca="false">((-0.078)*B35+(-0.207)*D35+(-0.477)*E35+(0.227)*F35)/ (-0.535)</f>
-        <v>0.0787706168224299</v>
+        <f aca="false">((0.078)*B35+(0.207)*D35+(0.477)*E35+(0.227)*F35)/ (0.989)</f>
+        <v>0.0635803842264914</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>383.603055555556</v>
@@ -2754,12 +2754,12 @@
         <v>78</v>
       </c>
       <c r="G36" s="0" t="n">
-        <f aca="false">((-0.078)*B36+(-0.218)*C36+(-0.477)*E36+(0.227)*F36)/(-0.546)</f>
-        <v>0.0639137728937729</v>
+        <f aca="false">((0.078)*B36+(0.218)*C36+(0.477)*E36+(0.227)*F36)/(1)</f>
+        <v>0.05305238</v>
       </c>
       <c r="H36" s="0" t="n">
-        <f aca="false">((-0.078)*B36+(-0.207)*D36+(-0.477)*E36+(0.227)*F36)/ (-0.535)</f>
-        <v>0.0671096635514019</v>
+        <f aca="false">((0.078)*B36+(0.207)*D36+(0.477)*E36+(0.227)*F36)/ (0.989)</f>
+        <v>0.0546603943377149</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>410.050277777778</v>
@@ -2803,12 +2803,12 @@
         <v>49</v>
       </c>
       <c r="G37" s="0" t="n">
-        <f aca="false">((-0.078)*B37+(-0.218)*C37+(-0.477)*E37+(0.227)*F37)/(-0.546)</f>
-        <v>-0.00831884615384615</v>
+        <f aca="false">((0.078)*B37+(0.218)*C37+(0.477)*E37+(0.227)*F37)/(1)</f>
+        <v>0.01662339</v>
       </c>
       <c r="H37" s="0" t="n">
-        <f aca="false">((-0.078)*B37+(-0.207)*D37+(-0.477)*E37+(0.227)*F37)/ (-0.535)</f>
-        <v>-0.00771011214953271</v>
+        <f aca="false">((0.078)*B37+(0.207)*D37+(0.477)*E37+(0.227)*F37)/ (0.989)</f>
+        <v>0.0172301011122346</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>134.468888888889</v>
@@ -2852,12 +2852,12 @@
         <v>68</v>
       </c>
       <c r="G38" s="0" t="n">
-        <f aca="false">((-0.078)*B38+(-0.218)*C38+(-0.477)*E38+(0.227)*F38)/(-0.546)</f>
-        <v>-0.00404961538461538</v>
+        <f aca="false">((0.078)*B38+(0.218)*C38+(0.477)*E38+(0.227)*F38)/(1)</f>
+        <v>0.01837781</v>
       </c>
       <c r="H38" s="0" t="n">
-        <f aca="false">((-0.078)*B38+(-0.207)*D38+(-0.477)*E38+(0.227)*F38)/ (-0.535)</f>
-        <v>-0.00247970093457944</v>
+        <f aca="false">((0.078)*B38+(0.207)*D38+(0.477)*E38+(0.227)*F38)/ (0.989)</f>
+        <v>0.0194765015166835</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>2315.50222222222</v>
@@ -2901,12 +2901,12 @@
         <v>19</v>
       </c>
       <c r="G39" s="0" t="n">
-        <f aca="false">((-0.078)*B39+(-0.218)*C39+(-0.477)*E39+(0.227)*F39)/(-0.546)</f>
-        <v>0.0238809523809524</v>
+        <f aca="false">((0.078)*B39+(0.218)*C39+(0.477)*E39+(0.227)*F39)/(1)</f>
+        <v>0.03368692</v>
       </c>
       <c r="H39" s="0" t="n">
-        <f aca="false">((-0.078)*B39+(-0.207)*D39+(-0.477)*E39+(0.227)*F39)/ (-0.535)</f>
-        <v>0.00292379439252336</v>
+        <f aca="false">((0.078)*B39+(0.207)*D39+(0.477)*E39+(0.227)*F39)/ (0.989)</f>
+        <v>0.0224592012133468</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>912.055833333333</v>
@@ -2950,12 +2950,12 @@
         <v>162</v>
       </c>
       <c r="G40" s="0" t="n">
-        <f aca="false">((-0.078)*B40+(-0.218)*C40+(-0.477)*E40+(0.227)*F40)/(-0.546)</f>
-        <v>-0.007285</v>
+        <f aca="false">((0.078)*B40+(0.218)*C40+(0.477)*E40+(0.227)*F40)/(1)</f>
+        <v>0.01051407</v>
       </c>
       <c r="H40" s="0" t="n">
-        <f aca="false">((-0.078)*B40+(-0.207)*D40+(-0.477)*E40+(0.227)*F40)/ (-0.535)</f>
-        <v>-0.00736317757009346</v>
+        <f aca="false">((0.078)*B40+(0.207)*D40+(0.477)*E40+(0.227)*F40)/ (0.989)</f>
+        <v>0.0106697472194136</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>593.220277777778</v>
@@ -2999,12 +2999,12 @@
         <v>68</v>
       </c>
       <c r="G41" s="0" t="n">
-        <f aca="false">((-0.078)*B41+(-0.218)*C41+(-0.477)*E41+(0.227)*F41)/(-0.546)</f>
-        <v>-0.0059897619047619</v>
+        <f aca="false">((0.078)*B41+(0.218)*C41+(0.477)*E41+(0.227)*F41)/(1)</f>
+        <v>0.01731849</v>
       </c>
       <c r="H41" s="0" t="n">
-        <f aca="false">((-0.078)*B41+(-0.207)*D41+(-0.477)*E41+(0.227)*F41)/ (-0.535)</f>
-        <v>-0.00544370093457944</v>
+        <f aca="false">((0.078)*B41+(0.207)*D41+(0.477)*E41+(0.227)*F41)/ (0.989)</f>
+        <v>0.0178731243680485</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>3038.70027777778</v>
@@ -3048,12 +3048,12 @@
         <v>49</v>
       </c>
       <c r="G42" s="0" t="n">
-        <f aca="false">((-0.078)*B42+(-0.218)*C42+(-0.477)*E42+(0.227)*F42)/(-0.546)</f>
-        <v>0.0240904395604396</v>
+        <f aca="false">((0.078)*B42+(0.218)*C42+(0.477)*E42+(0.227)*F42)/(1)</f>
+        <v>0.03431886</v>
       </c>
       <c r="H42" s="0" t="n">
-        <f aca="false">((-0.078)*B42+(-0.207)*D42+(-0.477)*E42+(0.227)*F42)/ (-0.535)</f>
-        <v>0.0252703177570093</v>
+        <f aca="false">((0.078)*B42+(0.207)*D42+(0.477)*E42+(0.227)*F42)/ (0.989)</f>
+        <v>0.0350708796764409</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>4815.88861111111</v>
@@ -3097,12 +3097,12 @@
         <v>174</v>
       </c>
       <c r="G43" s="0" t="n">
-        <f aca="false">((-0.078)*B43+(-0.218)*C43+(-0.477)*E43+(0.227)*F43)/(-0.546)</f>
-        <v>0.0696432600732601</v>
+        <f aca="false">((0.078)*B43+(0.218)*C43+(0.477)*E43+(0.227)*F43)/(1)</f>
+        <v>0.05665284</v>
       </c>
       <c r="H43" s="0" t="n">
-        <f aca="false">((-0.078)*B43+(-0.207)*D43+(-0.477)*E43+(0.227)*F43)/ (-0.535)</f>
-        <v>0.0735528037383178</v>
+        <f aca="false">((0.078)*B43+(0.207)*D43+(0.477)*E43+(0.227)*F43)/ (0.989)</f>
+        <v>0.0586232254802831</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>230.709444444444</v>
@@ -3146,12 +3146,12 @@
         <v>59</v>
       </c>
       <c r="G44" s="0" t="n">
-        <f aca="false">((-0.078)*B44+(-0.218)*C44+(-0.477)*E44+(0.227)*F44)/(-0.546)</f>
-        <v>-0.016470695970696</v>
+        <f aca="false">((0.078)*B44+(0.218)*C44+(0.477)*E44+(0.227)*F44)/(1)</f>
+        <v>0.01210892</v>
       </c>
       <c r="H44" s="0" t="n">
-        <f aca="false">((-0.078)*B44+(-0.207)*D44+(-0.477)*E44+(0.227)*F44)/ (-0.535)</f>
-        <v>-0.0174163551401869</v>
+        <f aca="false">((0.078)*B44+(0.207)*D44+(0.477)*E44+(0.227)*F44)/ (0.989)</f>
+        <v>0.0119152376137513</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>1119.42</v>
@@ -3195,12 +3195,12 @@
         <v>182</v>
       </c>
       <c r="G45" s="0" t="n">
-        <f aca="false">((-0.078)*B45+(-0.218)*C45+(-0.477)*E45+(0.227)*F45)/(-0.546)</f>
-        <v>0.060670347985348</v>
+        <f aca="false">((0.078)*B45+(0.218)*C45+(0.477)*E45+(0.227)*F45)/(1)</f>
+        <v>0.05387381</v>
       </c>
       <c r="H45" s="0" t="n">
-        <f aca="false">((-0.078)*B45+(-0.207)*D45+(-0.477)*E45+(0.227)*F45)/ (-0.535)</f>
-        <v>0.0631294392523365</v>
+        <f aca="false">((0.078)*B45+(0.207)*D45+(0.477)*E45+(0.227)*F45)/ (0.989)</f>
+        <v>0.0551284630940344</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>760.091666666667</v>
@@ -3244,12 +3244,12 @@
         <v>111</v>
       </c>
       <c r="G46" s="0" t="n">
-        <f aca="false">((-0.078)*B46+(-0.218)*C46+(-0.477)*E46+(0.227)*F46)/(-0.546)</f>
-        <v>-0.00388948717948718</v>
+        <f aca="false">((0.078)*B46+(0.218)*C46+(0.477)*E46+(0.227)*F46)/(1)</f>
+        <v>0.01861506</v>
       </c>
       <c r="H46" s="0" t="n">
-        <f aca="false">((-0.078)*B46+(-0.207)*D46+(-0.477)*E46+(0.227)*F46)/ (-0.535)</f>
-        <v>-0.00337981308411215</v>
+        <f aca="false">((0.078)*B46+(0.207)*D46+(0.477)*E46+(0.227)*F46)/ (0.989)</f>
+        <v>0.0191410717896866</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>3859.82166666667</v>
@@ -3293,12 +3293,12 @@
         <v>187</v>
       </c>
       <c r="G47" s="0" t="n">
-        <f aca="false">((-0.078)*B47+(-0.218)*C47+(-0.477)*E47+(0.227)*F47)/(-0.546)</f>
-        <v>0.0622413736263736</v>
+        <f aca="false">((0.078)*B47+(0.218)*C47+(0.477)*E47+(0.227)*F47)/(1)</f>
+        <v>0.05478607</v>
       </c>
       <c r="H47" s="0" t="n">
-        <f aca="false">((-0.078)*B47+(-0.207)*D47+(-0.477)*E47+(0.227)*F47)/ (-0.535)</f>
-        <v>0.0659987289719626</v>
+        <f aca="false">((0.078)*B47+(0.207)*D47+(0.477)*E47+(0.227)*F47)/ (0.989)</f>
+        <v>0.0567356926188069</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>275.270277777778</v>
@@ -3342,12 +3342,12 @@
         <v>191</v>
       </c>
       <c r="G48" s="0" t="n">
-        <f aca="false">((-0.078)*B48+(-0.218)*C48+(-0.477)*E48+(0.227)*F48)/(-0.546)</f>
-        <v>-0.0185219413919414</v>
+        <f aca="false">((0.078)*B48+(0.218)*C48+(0.477)*E48+(0.227)*F48)/(1)</f>
+        <v>0.0107574</v>
       </c>
       <c r="H48" s="0" t="n">
-        <f aca="false">((-0.078)*B48+(-0.207)*D48+(-0.477)*E48+(0.227)*F48)/ (-0.535)</f>
-        <v>-0.0194127289719626</v>
+        <f aca="false">((0.078)*B48+(0.207)*D48+(0.477)*E48+(0.227)*F48)/ (0.989)</f>
+        <v>0.0106011830131446</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>7454.53027777778</v>
@@ -3391,12 +3391,12 @@
         <v>193</v>
       </c>
       <c r="G49" s="0" t="n">
-        <f aca="false">((-0.078)*B49+(-0.218)*C49+(-0.477)*E49+(0.227)*F49)/(-0.546)</f>
-        <v>-0.0187337362637363</v>
+        <f aca="false">((0.078)*B49+(0.218)*C49+(0.477)*E49+(0.227)*F49)/(1)</f>
+        <v>0.01022862</v>
       </c>
       <c r="H49" s="0" t="n">
-        <f aca="false">((-0.078)*B49+(-0.207)*D49+(-0.477)*E49+(0.227)*F49)/ (-0.535)</f>
-        <v>-0.0191189158878505</v>
+        <f aca="false">((0.078)*B49+(0.207)*D49+(0.477)*E49+(0.227)*F49)/ (0.989)</f>
+        <v>0.0103423862487361</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>2390.77805555556</v>
@@ -3440,12 +3440,12 @@
         <v>78</v>
       </c>
       <c r="G50" s="0" t="n">
-        <f aca="false">((-0.078)*B50+(-0.218)*C50+(-0.477)*E50+(0.227)*F50)/(-0.546)</f>
-        <v>0.0558636813186813</v>
+        <f aca="false">((0.078)*B50+(0.218)*C50+(0.477)*E50+(0.227)*F50)/(1)</f>
+        <v>0.04865703</v>
       </c>
       <c r="H50" s="0" t="n">
-        <f aca="false">((-0.078)*B50+(-0.207)*D50+(-0.477)*E50+(0.227)*F50)/ (-0.535)</f>
-        <v>0.0558869719626168</v>
+        <f aca="false">((0.078)*B50+(0.207)*D50+(0.477)*E50+(0.227)*F50)/ (0.989)</f>
+        <v>0.0485894742163802</v>
       </c>
       <c r="I50" s="0" t="n">
         <v>555.086388888889</v>
@@ -3489,12 +3489,12 @@
         <v>68</v>
       </c>
       <c r="G51" s="0" t="n">
-        <f aca="false">((-0.078)*B51+(-0.218)*C51+(-0.477)*E51+(0.227)*F51)/(-0.546)</f>
-        <v>0.0958188644688645</v>
+        <f aca="false">((0.078)*B51+(0.218)*C51+(0.477)*E51+(0.227)*F51)/(1)</f>
+        <v>0.072906</v>
       </c>
       <c r="H51" s="0" t="n">
-        <f aca="false">((-0.078)*B51+(-0.207)*D51+(-0.477)*E51+(0.227)*F51)/ (-0.535)</f>
-        <v>0.0988891775700935</v>
+        <f aca="false">((0.078)*B51+(0.207)*D51+(0.477)*E51+(0.227)*F51)/ (0.989)</f>
+        <v>0.0743120424671385</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>1226.79777777778</v>
@@ -3538,12 +3538,12 @@
         <v>204</v>
       </c>
       <c r="G52" s="0" t="n">
-        <f aca="false">((-0.078)*B52+(-0.218)*C52+(-0.477)*E52+(0.227)*F52)/(-0.546)</f>
-        <v>-0.0178838461538462</v>
+        <f aca="false">((0.078)*B52+(0.218)*C52+(0.477)*E52+(0.227)*F52)/(1)</f>
+        <v>0.01109672</v>
       </c>
       <c r="H52" s="0" t="n">
-        <f aca="false">((-0.078)*B52+(-0.207)*D52+(-0.477)*E52+(0.227)*F52)/ (-0.535)</f>
-        <v>-0.0189837943925234</v>
+        <f aca="false">((0.078)*B52+(0.207)*D52+(0.477)*E52+(0.227)*F52)/ (0.989)</f>
+        <v>0.0108240343781598</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>1164.27805555556</v>
@@ -3587,12 +3587,12 @@
         <v>93</v>
       </c>
       <c r="G53" s="0" t="n">
-        <f aca="false">((-0.078)*B53+(-0.218)*C53+(-0.477)*E53+(0.227)*F53)/(-0.546)</f>
-        <v>0.0644312271062271</v>
+        <f aca="false">((0.078)*B53+(0.218)*C53+(0.477)*E53+(0.227)*F53)/(1)</f>
+        <v>0.05223623</v>
       </c>
       <c r="H53" s="0" t="n">
-        <f aca="false">((-0.078)*B53+(-0.207)*D53+(-0.477)*E53+(0.227)*F53)/ (-0.535)</f>
-        <v>0.0666310280373832</v>
+        <f aca="false">((0.078)*B53+(0.207)*D53+(0.477)*E53+(0.227)*F53)/ (0.989)</f>
+        <v>0.0532905763397371</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>240.651388888889</v>
@@ -3636,12 +3636,12 @@
         <v>211</v>
       </c>
       <c r="G54" s="0" t="n">
-        <f aca="false">((-0.078)*B54+(-0.218)*C54+(-0.477)*E54+(0.227)*F54)/(-0.546)</f>
-        <v>0.0662091025641026</v>
+        <f aca="false">((0.078)*B54+(0.218)*C54+(0.477)*E54+(0.227)*F54)/(1)</f>
+        <v>0.05718399</v>
       </c>
       <c r="H54" s="0" t="n">
-        <f aca="false">((-0.078)*B54+(-0.207)*D54+(-0.477)*E54+(0.227)*F54)/ (-0.535)</f>
-        <v>0.067716523364486</v>
+        <f aca="false">((0.078)*B54+(0.207)*D54+(0.477)*E54+(0.227)*F54)/ (0.989)</f>
+        <v>0.057899049544995</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>3890.5475</v>
@@ -3685,12 +3685,12 @@
         <v>216</v>
       </c>
       <c r="G55" s="0" t="n">
-        <f aca="false">((-0.078)*B55+(-0.218)*C55+(-0.477)*E55+(0.227)*F55)/(-0.546)</f>
-        <v>0.0651332967032967</v>
+        <f aca="false">((0.078)*B55+(0.218)*C55+(0.477)*E55+(0.227)*F55)/(1)</f>
+        <v>0.05637414</v>
       </c>
       <c r="H55" s="0" t="n">
-        <f aca="false">((-0.078)*B55+(-0.207)*D55+(-0.477)*E55+(0.227)*F55)/ (-0.535)</f>
-        <v>0.0665451028037383</v>
+        <f aca="false">((0.078)*B55+(0.207)*D55+(0.477)*E55+(0.227)*F55)/ (0.989)</f>
+        <v>0.0570404347826087</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>1472.15416666667</v>
@@ -3734,12 +3734,12 @@
         <v>111</v>
       </c>
       <c r="G56" s="0" t="n">
-        <f aca="false">((-0.078)*B56+(-0.218)*C56+(-0.477)*E56+(0.227)*F56)/(-0.546)</f>
-        <v>-0.0152469047619048</v>
+        <f aca="false">((0.078)*B56+(0.218)*C56+(0.477)*E56+(0.227)*F56)/(1)</f>
+        <v>0.01241391</v>
       </c>
       <c r="H56" s="0" t="n">
-        <f aca="false">((-0.078)*B56+(-0.207)*D56+(-0.477)*E56+(0.227)*F56)/ (-0.535)</f>
-        <v>-0.0159306355140187</v>
+        <f aca="false">((0.078)*B56+(0.207)*D56+(0.477)*E56+(0.227)*F56)/ (0.989)</f>
+        <v>0.012351698685541</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>52.3119444444444</v>
@@ -3783,12 +3783,12 @@
         <v>54</v>
       </c>
       <c r="G57" s="0" t="n">
-        <f aca="false">((-0.078)*B57+(-0.218)*C57+(-0.477)*E57+(0.227)*F57)/(-0.546)</f>
-        <v>-0.0113345238095238</v>
+        <f aca="false">((0.078)*B57+(0.218)*C57+(0.477)*E57+(0.227)*F57)/(1)</f>
+        <v>0.01484063</v>
       </c>
       <c r="H57" s="0" t="n">
-        <f aca="false">((-0.078)*B57+(-0.207)*D57+(-0.477)*E57+(0.227)*F57)/ (-0.535)</f>
-        <v>-0.0119300747663551</v>
+        <f aca="false">((0.078)*B57+(0.207)*D57+(0.477)*E57+(0.227)*F57)/ (0.989)</f>
+        <v>0.0148095955510617</v>
       </c>
       <c r="I57" s="0" t="n">
         <v>1670.61055555556</v>
@@ -3832,12 +3832,12 @@
         <v>34</v>
       </c>
       <c r="G58" s="0" t="n">
-        <f aca="false">((-0.078)*B58+(-0.218)*C58+(-0.477)*E58+(0.227)*F58)/(-0.546)</f>
-        <v>-0.0176841758241758</v>
+        <f aca="false">((0.078)*B58+(0.218)*C58+(0.477)*E58+(0.227)*F58)/(1)</f>
+        <v>0.01064278</v>
       </c>
       <c r="H58" s="0" t="n">
-        <f aca="false">((-0.078)*B58+(-0.207)*D58+(-0.477)*E58+(0.227)*F58)/ (-0.535)</f>
-        <v>-0.0180215140186916</v>
+        <f aca="false">((0.078)*B58+(0.207)*D58+(0.477)*E58+(0.227)*F58)/ (0.989)</f>
+        <v>0.0107753589484328</v>
       </c>
       <c r="I58" s="0" t="n">
         <v>9261.38444444444</v>
@@ -3881,12 +3881,12 @@
         <v>231</v>
       </c>
       <c r="G59" s="0" t="n">
-        <f aca="false">((-0.078)*B59+(-0.218)*C59+(-0.477)*E59+(0.227)*F59)/(-0.546)</f>
-        <v>-0.0108108058608059</v>
+        <f aca="false">((0.078)*B59+(0.218)*C59+(0.477)*E59+(0.227)*F59)/(1)</f>
+        <v>0.01508572</v>
       </c>
       <c r="H59" s="0" t="n">
-        <f aca="false">((-0.078)*B59+(-0.207)*D59+(-0.477)*E59+(0.227)*F59)/ (-0.535)</f>
-        <v>-0.0163260560747664</v>
+        <f aca="false">((0.078)*B59+(0.207)*D59+(0.477)*E59+(0.227)*F59)/ (0.989)</f>
+        <v>0.0123902730030334</v>
       </c>
       <c r="I59" s="0" t="n">
         <v>2565.895</v>
@@ -3930,12 +3930,12 @@
         <v>34</v>
       </c>
       <c r="G60" s="0" t="n">
-        <f aca="false">((-0.078)*B60+(-0.218)*C60+(-0.477)*E60+(0.227)*F60)/(-0.546)</f>
-        <v>0.0104943406593407</v>
+        <f aca="false">((0.078)*B60+(0.218)*C60+(0.477)*E60+(0.227)*F60)/(1)</f>
+        <v>0.02602825</v>
       </c>
       <c r="H60" s="0" t="n">
-        <f aca="false">((-0.078)*B60+(-0.207)*D60+(-0.477)*E60+(0.227)*F60)/ (-0.535)</f>
-        <v>0.0104017196261682</v>
+        <f aca="false">((0.078)*B60+(0.207)*D60+(0.477)*E60+(0.227)*F60)/ (0.989)</f>
+        <v>0.0261509201213347</v>
       </c>
       <c r="I60" s="0" t="n">
         <v>2075.28222222222</v>
@@ -3979,12 +3979,12 @@
         <v>130</v>
       </c>
       <c r="G61" s="0" t="n">
-        <f aca="false">((-0.078)*B61+(-0.218)*C61+(-0.477)*E61+(0.227)*F61)/(-0.546)</f>
-        <v>-0.00867564102564103</v>
+        <f aca="false">((0.078)*B61+(0.218)*C61+(0.477)*E61+(0.227)*F61)/(1)</f>
+        <v>0.01565224</v>
       </c>
       <c r="H61" s="0" t="n">
-        <f aca="false">((-0.078)*B61+(-0.207)*D61+(-0.477)*E61+(0.227)*F61)/ (-0.535)</f>
-        <v>-0.012356523364486</v>
+        <f aca="false">((0.078)*B61+(0.207)*D61+(0.477)*E61+(0.227)*F61)/ (0.989)</f>
+        <v>0.0139316481294237</v>
       </c>
       <c r="I61" s="0" t="n">
         <v>327.522777777778</v>
@@ -4028,12 +4028,12 @@
         <v>78</v>
       </c>
       <c r="G62" s="0" t="n">
-        <f aca="false">((-0.078)*B62+(-0.218)*C62+(-0.477)*E62+(0.227)*F62)/(-0.546)</f>
-        <v>0.0559688461538462</v>
+        <f aca="false">((0.078)*B62+(0.218)*C62+(0.477)*E62+(0.227)*F62)/(1)</f>
+        <v>0.04871445</v>
       </c>
       <c r="H62" s="0" t="n">
-        <f aca="false">((-0.078)*B62+(-0.207)*D62+(-0.477)*E62+(0.227)*F62)/ (-0.535)</f>
-        <v>0.0559710841121496</v>
+        <f aca="false">((0.078)*B62+(0.207)*D62+(0.477)*E62+(0.227)*F62)/ (0.989)</f>
+        <v>0.0486349747219414</v>
       </c>
       <c r="I62" s="0" t="n">
         <v>511.387777777778</v>
@@ -4077,12 +4077,12 @@
         <v>68</v>
       </c>
       <c r="G63" s="0" t="n">
-        <f aca="false">((-0.078)*B63+(-0.218)*C63+(-0.477)*E63+(0.227)*F63)/(-0.546)</f>
-        <v>0.0992855677655678</v>
+        <f aca="false">((0.078)*B63+(0.218)*C63+(0.477)*E63+(0.227)*F63)/(1)</f>
+        <v>0.07479882</v>
       </c>
       <c r="H63" s="0" t="n">
-        <f aca="false">((-0.078)*B63+(-0.207)*D63+(-0.477)*E63+(0.227)*F63)/ (-0.535)</f>
-        <v>0.103700112149533</v>
+        <f aca="false">((0.078)*B63+(0.207)*D63+(0.477)*E63+(0.227)*F63)/ (0.989)</f>
+        <v>0.0769145197168858</v>
       </c>
       <c r="I63" s="0" t="n">
         <v>800.326944444444</v>
@@ -4126,12 +4126,12 @@
         <v>59</v>
       </c>
       <c r="G64" s="0" t="n">
-        <f aca="false">((-0.078)*B64+(-0.218)*C64+(-0.477)*E64+(0.227)*F64)/(-0.546)</f>
-        <v>-0.00593150183150183</v>
+        <f aca="false">((0.078)*B64+(0.218)*C64+(0.477)*E64+(0.227)*F64)/(1)</f>
+        <v>0.01786332</v>
       </c>
       <c r="H64" s="0" t="n">
-        <f aca="false">((-0.078)*B64+(-0.207)*D64+(-0.477)*E64+(0.227)*F64)/ (-0.535)</f>
-        <v>-0.00553299065420561</v>
+        <f aca="false">((0.078)*B64+(0.207)*D64+(0.477)*E64+(0.227)*F64)/ (0.989)</f>
+        <v>0.0183435490394338</v>
       </c>
       <c r="I64" s="0" t="n">
         <v>1979.91027777778</v>
@@ -4175,12 +4175,12 @@
         <v>59</v>
       </c>
       <c r="G65" s="0" t="n">
-        <f aca="false">((-0.078)*B65+(-0.218)*C65+(-0.477)*E65+(0.227)*F65)/(-0.546)</f>
-        <v>-0.0086090293040293</v>
+        <f aca="false">((0.078)*B65+(0.218)*C65+(0.477)*E65+(0.227)*F65)/(1)</f>
+        <v>0.01640139</v>
       </c>
       <c r="H65" s="0" t="n">
-        <f aca="false">((-0.078)*B65+(-0.207)*D65+(-0.477)*E65+(0.227)*F65)/ (-0.535)</f>
-        <v>-0.00826557009345794</v>
+        <f aca="false">((0.078)*B65+(0.207)*D65+(0.477)*E65+(0.227)*F65)/ (0.989)</f>
+        <v>0.0168653589484328</v>
       </c>
       <c r="I65" s="0" t="n">
         <v>2660.99638888889</v>
@@ -4224,12 +4224,12 @@
         <v>111</v>
       </c>
       <c r="G66" s="0" t="n">
-        <f aca="false">((-0.078)*B66+(-0.218)*C66+(-0.477)*E66+(0.227)*F66)/(-0.546)</f>
-        <v>-0.0181688095238095</v>
+        <f aca="false">((0.078)*B66+(0.218)*C66+(0.477)*E66+(0.227)*F66)/(1)</f>
+        <v>0.01081855</v>
       </c>
       <c r="H66" s="0" t="n">
-        <f aca="false">((-0.078)*B66+(-0.207)*D66+(-0.477)*E66+(0.227)*F66)/ (-0.535)</f>
-        <v>-0.0181854579439252</v>
+        <f aca="false">((0.078)*B66+(0.207)*D66+(0.477)*E66+(0.227)*F66)/ (0.989)</f>
+        <v>0.0111319514661274</v>
       </c>
       <c r="I66" s="0" t="n">
         <v>3963.04027777778</v>
@@ -4273,12 +4273,12 @@
         <v>68</v>
       </c>
       <c r="G67" s="0" t="n">
-        <f aca="false">((-0.078)*B67+(-0.218)*C67+(-0.477)*E67+(0.227)*F67)/(-0.546)</f>
-        <v>-0.0110198351648352</v>
+        <f aca="false">((0.078)*B67+(0.218)*C67+(0.477)*E67+(0.227)*F67)/(1)</f>
+        <v>0.01457207</v>
       </c>
       <c r="H67" s="0" t="n">
-        <f aca="false">((-0.078)*B67+(-0.207)*D67+(-0.477)*E67+(0.227)*F67)/ (-0.535)</f>
-        <v>-0.0157305046728972</v>
+        <f aca="false">((0.078)*B67+(0.207)*D67+(0.477)*E67+(0.227)*F67)/ (0.989)</f>
+        <v>0.0123084732052578</v>
       </c>
       <c r="I67" s="0" t="n">
         <v>1685.2425</v>
@@ -4322,12 +4322,12 @@
         <v>93</v>
       </c>
       <c r="G68" s="0" t="n">
-        <f aca="false">((-0.078)*B68+(-0.218)*C68+(-0.477)*E68+(0.227)*F68)/(-0.546)</f>
-        <v>0.05699836996337</v>
+        <f aca="false">((0.078)*B68+(0.218)*C68+(0.477)*E68+(0.227)*F68)/(1)</f>
+        <v>0.04817789</v>
       </c>
       <c r="H68" s="0" t="n">
-        <f aca="false">((-0.078)*B68+(-0.207)*D68+(-0.477)*E68+(0.227)*F68)/ (-0.535)</f>
-        <v>0.0592001121495327</v>
+        <f aca="false">((0.078)*B68+(0.207)*D68+(0.477)*E68+(0.227)*F68)/ (0.989)</f>
+        <v>0.0492708190091001</v>
       </c>
       <c r="I68" s="0" t="n">
         <v>254.193055555556</v>
@@ -4371,12 +4371,12 @@
         <v>264</v>
       </c>
       <c r="G69" s="0" t="n">
-        <f aca="false">((-0.078)*B69+(-0.218)*C69+(-0.477)*E69+(0.227)*F69)/(-0.546)</f>
-        <v>0.10007021978022</v>
+        <f aca="false">((0.078)*B69+(0.218)*C69+(0.477)*E69+(0.227)*F69)/(1)</f>
+        <v>0.07331136</v>
       </c>
       <c r="H69" s="0" t="n">
-        <f aca="false">((-0.078)*B69+(-0.207)*D69+(-0.477)*E69+(0.227)*F69)/ (-0.535)</f>
-        <v>0.10072385046729</v>
+        <f aca="false">((0.078)*B69+(0.207)*D69+(0.477)*E69+(0.227)*F69)/ (0.989)</f>
+        <v>0.0733673205257836</v>
       </c>
       <c r="I69" s="0" t="n">
         <v>300.791111111111</v>
@@ -4420,12 +4420,12 @@
         <v>111</v>
       </c>
       <c r="G70" s="0" t="n">
-        <f aca="false">((-0.078)*B70+(-0.218)*C70+(-0.477)*E70+(0.227)*F70)/(-0.546)</f>
-        <v>-0.0163914652014652</v>
+        <f aca="false">((0.078)*B70+(0.218)*C70+(0.477)*E70+(0.227)*F70)/(1)</f>
+        <v>0.01178898</v>
       </c>
       <c r="H70" s="0" t="n">
-        <f aca="false">((-0.078)*B70+(-0.207)*D70+(-0.477)*E70+(0.227)*F70)/ (-0.535)</f>
-        <v>-0.0170948598130841</v>
+        <f aca="false">((0.078)*B70+(0.207)*D70+(0.477)*E70+(0.227)*F70)/ (0.989)</f>
+        <v>0.0117219110212336</v>
       </c>
       <c r="I70" s="0" t="n">
         <v>537.424444444445</v>
@@ -4469,12 +4469,12 @@
         <v>270</v>
       </c>
       <c r="G71" s="0" t="n">
-        <f aca="false">((-0.078)*B71+(-0.218)*C71+(-0.477)*E71+(0.227)*F71)/(-0.546)</f>
-        <v>-0.0125534249084249</v>
+        <f aca="false">((0.078)*B71+(0.218)*C71+(0.477)*E71+(0.227)*F71)/(1)</f>
+        <v>0.01412517</v>
       </c>
       <c r="H71" s="0" t="n">
-        <f aca="false">((-0.078)*B71+(-0.207)*D71+(-0.477)*E71+(0.227)*F71)/ (-0.535)</f>
-        <v>-0.0172956261682243</v>
+        <f aca="false">((0.078)*B71+(0.207)*D71+(0.477)*E71+(0.227)*F71)/ (0.989)</f>
+        <v>0.0118566026289181</v>
       </c>
       <c r="I71" s="0" t="n">
         <v>2341.27861111111</v>
@@ -4518,12 +4518,12 @@
         <v>275</v>
       </c>
       <c r="G72" s="0" t="n">
-        <f aca="false">((-0.078)*B72+(-0.218)*C72+(-0.477)*E72+(0.227)*F72)/(-0.546)</f>
-        <v>-0.00950613553113553</v>
+        <f aca="false">((0.078)*B72+(0.218)*C72+(0.477)*E72+(0.227)*F72)/(1)</f>
+        <v>0.00792117</v>
       </c>
       <c r="H72" s="0" t="n">
-        <f aca="false">((-0.078)*B72+(-0.207)*D72+(-0.477)*E72+(0.227)*F72)/ (-0.535)</f>
-        <v>-0.00987988785046729</v>
+        <f aca="false">((0.078)*B72+(0.207)*D72+(0.477)*E72+(0.227)*F72)/ (0.989)</f>
+        <v>0.00791282103134479</v>
       </c>
       <c r="I72" s="0" t="n">
         <v>871.348611111111</v>
@@ -4567,12 +4567,12 @@
         <v>278</v>
       </c>
       <c r="G73" s="0" t="n">
-        <f aca="false">((-0.078)*B73+(-0.218)*C73+(-0.477)*E73+(0.227)*F73)/(-0.546)</f>
-        <v>0.0996572527472528</v>
+        <f aca="false">((0.078)*B73+(0.218)*C73+(0.477)*E73+(0.227)*F73)/(1)</f>
+        <v>0.07311312</v>
       </c>
       <c r="H73" s="0" t="n">
-        <f aca="false">((-0.078)*B73+(-0.207)*D73+(-0.477)*E73+(0.227)*F73)/ (-0.535)</f>
-        <v>0.102407214953271</v>
+        <f aca="false">((0.078)*B73+(0.207)*D73+(0.477)*E73+(0.227)*F73)/ (0.989)</f>
+        <v>0.0743054802831143</v>
       </c>
       <c r="I73" s="0" t="n">
         <v>320.050555555555</v>
@@ -4616,12 +4616,12 @@
         <v>111</v>
       </c>
       <c r="G74" s="0" t="n">
-        <f aca="false">((-0.078)*B74+(-0.218)*C74+(-0.477)*E74+(0.227)*F74)/(-0.546)</f>
-        <v>0.0670071794871795</v>
+        <f aca="false">((0.078)*B74+(0.218)*C74+(0.477)*E74+(0.227)*F74)/(1)</f>
+        <v>0.05732464</v>
       </c>
       <c r="H74" s="0" t="n">
-        <f aca="false">((-0.078)*B74+(-0.207)*D74+(-0.477)*E74+(0.227)*F74)/ (-0.535)</f>
-        <v>0.0695733457943925</v>
+        <f aca="false">((0.078)*B74+(0.207)*D74+(0.477)*E74+(0.227)*F74)/ (0.989)</f>
+        <v>0.0586051162790698</v>
       </c>
       <c r="I74" s="0" t="n">
         <v>262.884722222222</v>
@@ -4665,12 +4665,12 @@
         <v>93</v>
       </c>
       <c r="G75" s="0" t="n">
-        <f aca="false">((-0.078)*B75+(-0.218)*C75+(-0.477)*E75+(0.227)*F75)/(-0.546)</f>
-        <v>0.0639077655677656</v>
+        <f aca="false">((0.078)*B75+(0.218)*C75+(0.477)*E75+(0.227)*F75)/(1)</f>
+        <v>0.05195042</v>
       </c>
       <c r="H75" s="0" t="n">
-        <f aca="false">((-0.078)*B75+(-0.207)*D75+(-0.477)*E75+(0.227)*F75)/ (-0.535)</f>
-        <v>0.0663753831775701</v>
+        <f aca="false">((0.078)*B75+(0.207)*D75+(0.477)*E75+(0.227)*F75)/ (0.989)</f>
+        <v>0.0531522851365015</v>
       </c>
       <c r="I75" s="0" t="n">
         <v>307.9175</v>
@@ -4714,12 +4714,12 @@
         <v>270</v>
       </c>
       <c r="G76" s="0" t="n">
-        <f aca="false">((-0.078)*B76+(-0.218)*C76+(-0.477)*E76+(0.227)*F76)/(-0.546)</f>
-        <v>0.0608271428571429</v>
+        <f aca="false">((0.078)*B76+(0.218)*C76+(0.477)*E76+(0.227)*F76)/(1)</f>
+        <v>0.05419096</v>
       </c>
       <c r="H76" s="0" t="n">
-        <f aca="false">((-0.078)*B76+(-0.207)*D76+(-0.477)*E76+(0.227)*F76)/ (-0.535)</f>
-        <v>0.0645902429906542</v>
+        <f aca="false">((0.078)*B76+(0.207)*D76+(0.477)*E76+(0.227)*F76)/ (0.989)</f>
+        <v>0.0561528008088979</v>
       </c>
       <c r="I76" s="0" t="n">
         <v>238.313888888889</v>
@@ -4763,12 +4763,12 @@
         <v>286</v>
       </c>
       <c r="G77" s="0" t="n">
-        <f aca="false">((-0.078)*B77+(-0.218)*C77+(-0.477)*E77+(0.227)*F77)/(-0.546)</f>
-        <v>0.0153081501831502</v>
+        <f aca="false">((0.078)*B77+(0.218)*C77+(0.477)*E77+(0.227)*F77)/(1)</f>
+        <v>0.02910151</v>
       </c>
       <c r="H77" s="0" t="n">
-        <f aca="false">((-0.078)*B77+(-0.207)*D77+(-0.477)*E77+(0.227)*F77)/ (-0.535)</f>
-        <v>0.0153627476635514</v>
+        <f aca="false">((0.078)*B77+(0.207)*D77+(0.477)*E77+(0.227)*F77)/ (0.989)</f>
+        <v>0.029284459049545</v>
       </c>
       <c r="I77" s="0" t="n">
         <v>2970.37972222222</v>
@@ -4812,12 +4812,12 @@
         <v>93</v>
       </c>
       <c r="G78" s="0" t="n">
-        <f aca="false">((-0.078)*B78+(-0.218)*C78+(-0.477)*E78+(0.227)*F78)/(-0.546)</f>
-        <v>-0.00501399267399268</v>
+        <f aca="false">((0.078)*B78+(0.218)*C78+(0.477)*E78+(0.227)*F78)/(1)</f>
+        <v>0.01431914</v>
       </c>
       <c r="H78" s="0" t="n">
-        <f aca="false">((-0.078)*B78+(-0.207)*D78+(-0.477)*E78+(0.227)*F78)/ (-0.535)</f>
-        <v>-0.00563078504672897</v>
+        <f aca="false">((0.078)*B78+(0.207)*D78+(0.477)*E78+(0.227)*F78)/ (0.989)</f>
+        <v>0.0142005156723964</v>
       </c>
       <c r="I78" s="0" t="n">
         <v>3032.47805555555</v>
@@ -4861,12 +4861,12 @@
         <v>111</v>
       </c>
       <c r="G79" s="0" t="n">
-        <f aca="false">((-0.078)*B79+(-0.218)*C79+(-0.477)*E79+(0.227)*F79)/(-0.546)</f>
-        <v>0.00980549450549451</v>
+        <f aca="false">((0.078)*B79+(0.218)*C79+(0.477)*E79+(0.227)*F79)/(1)</f>
+        <v>0.02609252</v>
       </c>
       <c r="H79" s="0" t="n">
-        <f aca="false">((-0.078)*B79+(-0.207)*D79+(-0.477)*E79+(0.227)*F79)/ (-0.535)</f>
-        <v>0.00967730841121495</v>
+        <f aca="false">((0.078)*B79+(0.207)*D79+(0.477)*E79+(0.227)*F79)/ (0.989)</f>
+        <v>0.02620432760364</v>
       </c>
       <c r="I79" s="0" t="n">
         <v>1585.9225</v>
@@ -4910,12 +4910,12 @@
         <v>296</v>
       </c>
       <c r="G80" s="0" t="n">
-        <f aca="false">((-0.078)*B80+(-0.218)*C80+(-0.477)*E80+(0.227)*F80)/(-0.546)</f>
-        <v>-0.0131565384615385</v>
+        <f aca="false">((0.078)*B80+(0.218)*C80+(0.477)*E80+(0.227)*F80)/(1)</f>
+        <v>0.01006399</v>
       </c>
       <c r="H80" s="0" t="n">
-        <f aca="false">((-0.078)*B80+(-0.207)*D80+(-0.477)*E80+(0.227)*F80)/ (-0.535)</f>
-        <v>-0.0141300373831776</v>
+        <f aca="false">((0.078)*B80+(0.207)*D80+(0.477)*E80+(0.227)*F80)/ (0.989)</f>
+        <v>0.00979564206268959</v>
       </c>
       <c r="I80" s="0" t="n">
         <v>1058.49388888889</v>
@@ -4959,12 +4959,12 @@
         <v>111</v>
       </c>
       <c r="G81" s="0" t="n">
-        <f aca="false">((-0.078)*B81+(-0.218)*C81+(-0.477)*E81+(0.227)*F81)/(-0.546)</f>
-        <v>-0.0181688095238095</v>
+        <f aca="false">((0.078)*B81+(0.218)*C81+(0.477)*E81+(0.227)*F81)/(1)</f>
+        <v>0.01081855</v>
       </c>
       <c r="H81" s="0" t="n">
-        <f aca="false">((-0.078)*B81+(-0.207)*D81+(-0.477)*E81+(0.227)*F81)/ (-0.535)</f>
-        <v>-0.0181854579439252</v>
+        <f aca="false">((0.078)*B81+(0.207)*D81+(0.477)*E81+(0.227)*F81)/ (0.989)</f>
+        <v>0.0111319514661274</v>
       </c>
       <c r="I81" s="0" t="n">
         <v>4382.32166666667</v>
@@ -5008,12 +5008,12 @@
         <v>34</v>
       </c>
       <c r="G82" s="0" t="n">
-        <f aca="false">((-0.078)*B82+(-0.218)*C82+(-0.477)*E82+(0.227)*F82)/(-0.546)</f>
-        <v>-0.0182012454212454</v>
+        <f aca="false">((0.078)*B82+(0.218)*C82+(0.477)*E82+(0.227)*F82)/(1)</f>
+        <v>0.01036046</v>
       </c>
       <c r="H82" s="0" t="n">
-        <f aca="false">((-0.078)*B82+(-0.207)*D82+(-0.477)*E82+(0.227)*F82)/ (-0.535)</f>
-        <v>-0.0182185607476636</v>
+        <f aca="false">((0.078)*B82+(0.207)*D82+(0.477)*E82+(0.227)*F82)/ (0.989)</f>
+        <v>0.0106687664307381</v>
       </c>
       <c r="I82" s="0" t="n">
         <v>6227.56222222222</v>
@@ -5057,12 +5057,12 @@
         <v>34</v>
       </c>
       <c r="G83" s="0" t="n">
-        <f aca="false">((-0.078)*B83+(-0.218)*C83+(-0.477)*E83+(0.227)*F83)/(-0.546)</f>
-        <v>-0.0182212454212454</v>
+        <f aca="false">((0.078)*B83+(0.218)*C83+(0.477)*E83+(0.227)*F83)/(1)</f>
+        <v>0.01034954</v>
       </c>
       <c r="H83" s="0" t="n">
-        <f aca="false">((-0.078)*B83+(-0.207)*D83+(-0.477)*E83+(0.227)*F83)/ (-0.535)</f>
-        <v>-0.0182428411214953</v>
+        <f aca="false">((0.078)*B83+(0.207)*D83+(0.477)*E83+(0.227)*F83)/ (0.989)</f>
+        <v>0.0106556319514661</v>
       </c>
       <c r="I83" s="0" t="n">
         <v>4423.29944444445</v>
@@ -5106,12 +5106,12 @@
         <v>34</v>
       </c>
       <c r="G84" s="0" t="n">
-        <f aca="false">((-0.078)*B84+(-0.218)*C84+(-0.477)*E84+(0.227)*F84)/(-0.546)</f>
-        <v>-0.0182012454212454</v>
+        <f aca="false">((0.078)*B84+(0.218)*C84+(0.477)*E84+(0.227)*F84)/(1)</f>
+        <v>0.01036046</v>
       </c>
       <c r="H84" s="0" t="n">
-        <f aca="false">((-0.078)*B84+(-0.207)*D84+(-0.477)*E84+(0.227)*F84)/ (-0.535)</f>
-        <v>-0.0182185607476636</v>
+        <f aca="false">((0.078)*B84+(0.207)*D84+(0.477)*E84+(0.227)*F84)/ (0.989)</f>
+        <v>0.0106687664307381</v>
       </c>
       <c r="I84" s="0" t="n">
         <v>4022.14388888889</v>
@@ -5155,12 +5155,12 @@
         <v>59</v>
       </c>
       <c r="G85" s="0" t="n">
-        <f aca="false">((-0.078)*B85+(-0.218)*C85+(-0.477)*E85+(0.227)*F85)/(-0.546)</f>
-        <v>-0.0115281501831502</v>
+        <f aca="false">((0.078)*B85+(0.218)*C85+(0.477)*E85+(0.227)*F85)/(1)</f>
+        <v>0.01480755</v>
       </c>
       <c r="H85" s="0" t="n">
-        <f aca="false">((-0.078)*B85+(-0.207)*D85+(-0.477)*E85+(0.227)*F85)/ (-0.535)</f>
-        <v>-0.0111840934579439</v>
+        <f aca="false">((0.078)*B85+(0.207)*D85+(0.477)*E85+(0.227)*F85)/ (0.989)</f>
+        <v>0.0152865824064712</v>
       </c>
       <c r="I85" s="0" t="n">
         <v>2016.81416666667</v>
@@ -5204,12 +5204,12 @@
         <v>130</v>
       </c>
       <c r="G86" s="0" t="n">
-        <f aca="false">((-0.078)*B86+(-0.218)*C86+(-0.477)*E86+(0.227)*F86)/(-0.546)</f>
-        <v>0.0275282051282051</v>
+        <f aca="false">((0.078)*B86+(0.218)*C86+(0.477)*E86+(0.227)*F86)/(1)</f>
+        <v>0.03541954</v>
       </c>
       <c r="H86" s="0" t="n">
-        <f aca="false">((-0.078)*B86+(-0.207)*D86+(-0.477)*E86+(0.227)*F86)/ (-0.535)</f>
-        <v>0.00159930841121495</v>
+        <f aca="false">((0.078)*B86+(0.207)*D86+(0.477)*E86+(0.227)*F86)/ (0.989)</f>
+        <v>0.0214810616784631</v>
       </c>
       <c r="I86" s="0" t="n">
         <v>546.275</v>
@@ -5253,12 +5253,12 @@
         <v>111</v>
       </c>
       <c r="G87" s="0" t="n">
-        <f aca="false">((-0.078)*B87+(-0.218)*C87+(-0.477)*E87+(0.227)*F87)/(-0.546)</f>
-        <v>-0.00862047619047619</v>
+        <f aca="false">((0.078)*B87+(0.218)*C87+(0.477)*E87+(0.227)*F87)/(1)</f>
+        <v>0.01603194</v>
       </c>
       <c r="H87" s="0" t="n">
-        <f aca="false">((-0.078)*B87+(-0.207)*D87+(-0.477)*E87+(0.227)*F87)/ (-0.535)</f>
-        <v>-0.00873596261682243</v>
+        <f aca="false">((0.078)*B87+(0.207)*D87+(0.477)*E87+(0.227)*F87)/ (0.989)</f>
+        <v>0.0162436602628918</v>
       </c>
       <c r="I87" s="0" t="n">
         <v>1356.98</v>
@@ -5302,12 +5302,12 @@
         <v>204</v>
       </c>
       <c r="G88" s="0" t="n">
-        <f aca="false">((-0.078)*B88+(-0.218)*C88+(-0.477)*E88+(0.227)*F88)/(-0.546)</f>
-        <v>-0.0156139926739927</v>
+        <f aca="false">((0.078)*B88+(0.218)*C88+(0.477)*E88+(0.227)*F88)/(1)</f>
+        <v>0.01233606</v>
       </c>
       <c r="H88" s="0" t="n">
-        <f aca="false">((-0.078)*B88+(-0.207)*D88+(-0.477)*E88+(0.227)*F88)/ (-0.535)</f>
-        <v>-0.0165637196261682</v>
+        <f aca="false">((0.078)*B88+(0.207)*D88+(0.477)*E88+(0.227)*F88)/ (0.989)</f>
+        <v>0.0121331749241658</v>
       </c>
       <c r="I88" s="0" t="n">
         <v>2738.57861111111</v>
@@ -5351,12 +5351,12 @@
         <v>130</v>
       </c>
       <c r="G89" s="0" t="n">
-        <f aca="false">((-0.078)*B89+(-0.218)*C89+(-0.477)*E89+(0.227)*F89)/(-0.546)</f>
-        <v>-0.00850838827838828</v>
+        <f aca="false">((0.078)*B89+(0.218)*C89+(0.477)*E89+(0.227)*F89)/(1)</f>
+        <v>0.01574356</v>
       </c>
       <c r="H89" s="0" t="n">
-        <f aca="false">((-0.078)*B89+(-0.207)*D89+(-0.477)*E89+(0.227)*F89)/ (-0.535)</f>
-        <v>-0.0121858317757009</v>
+        <f aca="false">((0.078)*B89+(0.207)*D89+(0.477)*E89+(0.227)*F89)/ (0.989)</f>
+        <v>0.0140239838220425</v>
       </c>
       <c r="I89" s="0" t="n">
         <v>686.612222222222</v>
@@ -5400,12 +5400,12 @@
         <v>34</v>
       </c>
       <c r="G90" s="0" t="n">
-        <f aca="false">((-0.078)*B90+(-0.218)*C90+(-0.477)*E90+(0.227)*F90)/(-0.546)</f>
-        <v>-0.018202673992674</v>
+        <f aca="false">((0.078)*B90+(0.218)*C90+(0.477)*E90+(0.227)*F90)/(1)</f>
+        <v>0.01035968</v>
       </c>
       <c r="H90" s="0" t="n">
-        <f aca="false">((-0.078)*B90+(-0.207)*D90+(-0.477)*E90+(0.227)*F90)/ (-0.535)</f>
-        <v>-0.0182200186915888</v>
+        <f aca="false">((0.078)*B90+(0.207)*D90+(0.477)*E90+(0.227)*F90)/ (0.989)</f>
+        <v>0.0106679777553084</v>
       </c>
       <c r="I90" s="0" t="n">
         <v>3292.90138888889</v>
@@ -5449,12 +5449,12 @@
         <v>261</v>
       </c>
       <c r="G91" s="0" t="n">
-        <f aca="false">((-0.078)*B91+(-0.218)*C91+(-0.477)*E91+(0.227)*F91)/(-0.546)</f>
-        <v>-0.000887619047619048</v>
+        <f aca="false">((0.078)*B91+(0.218)*C91+(0.477)*E91+(0.227)*F91)/(1)</f>
+        <v>0.00321546</v>
       </c>
       <c r="H91" s="0" t="n">
-        <f aca="false">((-0.078)*B91+(-0.207)*D91+(-0.477)*E91+(0.227)*F91)/ (-0.535)</f>
-        <v>-0.00108416822429907</v>
+        <f aca="false">((0.078)*B91+(0.207)*D91+(0.477)*E91+(0.227)*F91)/ (0.989)</f>
+        <v>0.00315477249747219</v>
       </c>
       <c r="I91" s="0" t="n">
         <v>661.900833333333</v>
@@ -5500,6 +5500,36 @@
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>